<commit_message>
make pt15 pt13 more robust
</commit_message>
<xml_diff>
--- a/rapports/Classeur1.xlsx
+++ b/rapports/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MASSON\Desktop\STAGE_EPINOCHE\moduleMorpho\rapports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B95888-76FC-4D59-A8AB-CE49BF53ED4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D59C96A-6A37-4D6A-A4CF-43AFE63DD1FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B8B69406-25B6-432A-850C-CDEAD3F40E8A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
   <si>
     <t>pt3</t>
   </si>
@@ -552,14 +552,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E05084-3E91-45D4-8B21-9364EA312050}">
-  <dimension ref="B1:K45"/>
+  <dimension ref="B1:K60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1251,6 +1252,235 @@
       <c r="J45" s="12"/>
       <c r="K45" s="11"/>
     </row>
+    <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>1074</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>1077</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>1086</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>1099</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>1107</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="11"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>1119</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
+        <v>1124</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4">
+        <v>1126</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>1129</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
+        <v>1145</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="11"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
+        <v>1149</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+    </row>
+    <row r="60" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="7">
+        <v>1152</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>